<commit_message>
Adding ExternalMergeSort.java and tasks
</commit_message>
<xml_diff>
--- a/TasksList/TasksList.xlsx
+++ b/TasksList/TasksList.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="FileProblems" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -114,6 +115,15 @@
   </si>
   <si>
     <t>programs\backtracking\QueensProblem.java</t>
+  </si>
+  <si>
+    <t>Find an eff algo that returns the Kth Line from end of the file.</t>
+  </si>
+  <si>
+    <t>Find an eff algo that sorts a given txt file of numbers.</t>
+  </si>
+  <si>
+    <t>Find an eff algo that search for a record in a given txt file.</t>
   </si>
 </sst>
 </file>
@@ -155,7 +165,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -175,6 +185,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,4 +611,71 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7">
+        <v>42620</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>